<commit_message>
Minor edits to clarify location names
</commit_message>
<xml_diff>
--- a/Retail_ABM_Model_Files/Agents smartlist.xlsx
+++ b/Retail_ABM_Model_Files/Agents smartlist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yeonjinjung/Desktop/ABM_Retail/ABM_retail_github/ABM_Model_Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yeonjinjung/Desktop/ABM_Retail/Retail_ABM_github/Retail_ABM_Model_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B316E12-6B30-C94E-83C7-39F99D5E95A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063736CA-EE71-F549-AEA5-4EE44DE28F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{A492ED55-7B61-7A40-9281-1C4409A3562C}"/>
   </bookViews>
@@ -77,9 +77,6 @@
     <t>refrigerator</t>
   </si>
   <si>
-    <t>dry-display</t>
-  </si>
-  <si>
     <t>runner</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
     <t xml:space="preserve">door </t>
   </si>
   <si>
-    <t>wet-display</t>
-  </si>
-  <si>
     <t>Out</t>
   </si>
   <si>
@@ -128,9 +122,6 @@
     <t>employee</t>
   </si>
   <si>
-    <t>dry-display-shelf</t>
-  </si>
-  <si>
     <t>consumer-scale</t>
   </si>
   <si>
@@ -267,6 +258,15 @@
   </si>
   <si>
     <t>z-default-water</t>
+  </si>
+  <si>
+    <t>dry-shelf</t>
+  </si>
+  <si>
+    <t>wet-display-area</t>
+  </si>
+  <si>
+    <t>dry-display-area</t>
   </si>
 </sst>
 </file>
@@ -357,9 +357,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -397,7 +397,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -503,7 +503,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -645,7 +645,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -655,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B75B978-DDD2-AE40-A7B1-ABB229DAD62A}">
   <dimension ref="A1:O69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="141" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -674,10 +674,10 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -692,22 +692,22 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -736,7 +736,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -745,7 +745,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -753,7 +753,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C3">
         <v>42</v>
@@ -774,7 +774,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -783,7 +783,7 @@
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -793,7 +793,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>42</v>
@@ -814,7 +814,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J4">
         <v>2</v>
@@ -823,7 +823,7 @@
         <v>1</v>
       </c>
       <c r="L4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -852,7 +852,7 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J5">
         <v>2</v>
@@ -861,7 +861,7 @@
         <v>2</v>
       </c>
       <c r="L5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -890,7 +890,7 @@
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -899,7 +899,7 @@
         <v>2</v>
       </c>
       <c r="L6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -907,7 +907,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>42</v>
@@ -928,7 +928,7 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J7">
         <v>2</v>
@@ -937,7 +937,7 @@
         <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -945,7 +945,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8">
         <v>42</v>
@@ -966,7 +966,7 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -975,7 +975,7 @@
         <v>1</v>
       </c>
       <c r="L8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -983,7 +983,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C9">
         <v>49</v>
@@ -1004,7 +1004,7 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -1013,7 +1013,7 @@
         <v>2</v>
       </c>
       <c r="L9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -1042,7 +1042,7 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J10">
         <v>1</v>
@@ -1051,7 +1051,7 @@
         <v>2</v>
       </c>
       <c r="L10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -1080,7 +1080,7 @@
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -1089,7 +1089,7 @@
         <v>1</v>
       </c>
       <c r="L11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -1097,7 +1097,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12">
         <v>44</v>
@@ -1118,7 +1118,7 @@
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J12">
         <v>5</v>
@@ -1127,7 +1127,7 @@
         <v>1</v>
       </c>
       <c r="L12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -1135,7 +1135,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13">
         <v>21</v>
@@ -1156,7 +1156,7 @@
         <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="J13">
         <v>4</v>
@@ -1165,7 +1165,7 @@
         <v>1</v>
       </c>
       <c r="L13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -1173,7 +1173,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="C14">
         <v>15</v>
@@ -1194,7 +1194,7 @@
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="J14">
         <v>3</v>
@@ -1203,7 +1203,7 @@
         <v>1</v>
       </c>
       <c r="L14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
@@ -1211,7 +1211,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C15">
         <v>16</v>
@@ -1232,7 +1232,7 @@
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="J15">
         <v>1</v>
@@ -1241,7 +1241,7 @@
         <v>1</v>
       </c>
       <c r="L15" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -1249,7 +1249,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16">
         <v>40</v>
@@ -1270,7 +1270,7 @@
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J16">
         <v>1</v>
@@ -1279,7 +1279,7 @@
         <v>1</v>
       </c>
       <c r="L16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -1287,7 +1287,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C17">
         <v>37</v>
@@ -1308,7 +1308,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J17">
         <v>1</v>
@@ -1317,7 +1317,7 @@
         <v>1</v>
       </c>
       <c r="L17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -1325,7 +1325,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C18">
         <v>37</v>
@@ -1346,7 +1346,7 @@
         <v>1</v>
       </c>
       <c r="I18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J18">
         <v>4</v>
@@ -1355,7 +1355,7 @@
         <v>1</v>
       </c>
       <c r="L18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -1363,7 +1363,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C19">
         <v>10</v>
@@ -1384,7 +1384,7 @@
         <v>1</v>
       </c>
       <c r="I19" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J19">
         <v>1</v>
@@ -1393,7 +1393,7 @@
         <v>1</v>
       </c>
       <c r="L19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -1401,7 +1401,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C20">
         <v>6</v>
@@ -1422,7 +1422,7 @@
         <v>1</v>
       </c>
       <c r="I20" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J20">
         <v>5</v>
@@ -1431,7 +1431,7 @@
         <v>1</v>
       </c>
       <c r="L20" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -1439,7 +1439,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="C21">
         <v>15</v>
@@ -1460,7 +1460,7 @@
         <v>1</v>
       </c>
       <c r="I21" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="J21">
         <v>3</v>
@@ -1469,7 +1469,7 @@
         <v>1</v>
       </c>
       <c r="L21" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -1477,7 +1477,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="C22">
         <v>15</v>
@@ -1498,7 +1498,7 @@
         <v>1</v>
       </c>
       <c r="I22" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="J22">
         <v>3</v>
@@ -1507,7 +1507,7 @@
         <v>1</v>
       </c>
       <c r="L22" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -1515,7 +1515,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="C23">
         <v>15</v>
@@ -1536,7 +1536,7 @@
         <v>1</v>
       </c>
       <c r="I23" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="J23">
         <v>3</v>
@@ -1545,7 +1545,7 @@
         <v>1</v>
       </c>
       <c r="L23" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -1553,7 +1553,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="C24">
         <v>26</v>
@@ -1574,7 +1574,7 @@
         <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="J24">
         <v>3</v>
@@ -1583,7 +1583,7 @@
         <v>1</v>
       </c>
       <c r="L24" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
@@ -1591,7 +1591,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="C25">
         <v>26</v>
@@ -1612,7 +1612,7 @@
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="J25">
         <v>3</v>
@@ -1621,7 +1621,7 @@
         <v>1</v>
       </c>
       <c r="L25" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
@@ -1629,7 +1629,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="C26">
         <v>26</v>
@@ -1650,7 +1650,7 @@
         <v>1</v>
       </c>
       <c r="I26" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="J26">
         <v>3</v>
@@ -1659,7 +1659,7 @@
         <v>1</v>
       </c>
       <c r="L26" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
@@ -1667,7 +1667,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="C27">
         <v>26</v>
@@ -1688,7 +1688,7 @@
         <v>1</v>
       </c>
       <c r="I27" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="J27">
         <v>3</v>
@@ -1697,7 +1697,7 @@
         <v>1</v>
       </c>
       <c r="L27" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
@@ -1705,7 +1705,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="C28">
         <v>12</v>
@@ -1726,7 +1726,7 @@
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="J28">
         <v>3</v>
@@ -1735,7 +1735,7 @@
         <v>1</v>
       </c>
       <c r="L28" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -1743,7 +1743,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="C29">
         <v>23</v>
@@ -1764,7 +1764,7 @@
         <v>1</v>
       </c>
       <c r="I29" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="J29">
         <v>3</v>
@@ -1773,7 +1773,7 @@
         <v>1</v>
       </c>
       <c r="L29" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
@@ -1781,7 +1781,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="C30">
         <v>34</v>
@@ -1802,7 +1802,7 @@
         <v>1</v>
       </c>
       <c r="I30" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="J30">
         <v>3</v>
@@ -1811,7 +1811,7 @@
         <v>1</v>
       </c>
       <c r="L30" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
@@ -1819,7 +1819,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="C31">
         <v>42</v>
@@ -1840,7 +1840,7 @@
         <v>1</v>
       </c>
       <c r="I31" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="J31">
         <v>3</v>
@@ -1849,7 +1849,7 @@
         <v>1</v>
       </c>
       <c r="L31" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
@@ -1857,7 +1857,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="C32">
         <v>38</v>
@@ -1878,7 +1878,7 @@
         <v>1</v>
       </c>
       <c r="I32" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="J32">
         <v>3</v>
@@ -1887,7 +1887,7 @@
         <v>1</v>
       </c>
       <c r="L32" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
@@ -1895,7 +1895,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C33">
         <v>49</v>
@@ -1916,7 +1916,7 @@
         <v>1</v>
       </c>
       <c r="I33" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J33">
         <v>2</v>
@@ -1925,7 +1925,7 @@
         <v>2</v>
       </c>
       <c r="L33" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
@@ -1933,7 +1933,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C34">
         <v>42</v>
@@ -1954,7 +1954,7 @@
         <v>1</v>
       </c>
       <c r="I34" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J34">
         <v>1</v>
@@ -1963,7 +1963,7 @@
         <v>1</v>
       </c>
       <c r="L34" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
@@ -1971,7 +1971,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C35">
         <v>31</v>
@@ -1992,7 +1992,7 @@
         <v>1</v>
       </c>
       <c r="I35" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="J35">
         <v>1</v>
@@ -2001,7 +2001,7 @@
         <v>1</v>
       </c>
       <c r="L35" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
@@ -2009,7 +2009,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C36">
         <v>11</v>
@@ -2030,7 +2030,7 @@
         <v>1</v>
       </c>
       <c r="I36" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="J36">
         <v>1</v>
@@ -2039,7 +2039,7 @@
         <v>1</v>
       </c>
       <c r="L36" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
@@ -2047,7 +2047,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C37">
         <v>4</v>
@@ -2068,7 +2068,7 @@
         <v>1</v>
       </c>
       <c r="I37" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J37">
         <v>2</v>
@@ -2077,7 +2077,7 @@
         <v>3</v>
       </c>
       <c r="L37" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
@@ -2085,7 +2085,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C38">
         <v>4</v>
@@ -2106,7 +2106,7 @@
         <v>1</v>
       </c>
       <c r="I38" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J38">
         <v>2</v>
@@ -2115,7 +2115,7 @@
         <v>3</v>
       </c>
       <c r="L38" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
@@ -2123,7 +2123,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C39">
         <v>4</v>
@@ -2144,7 +2144,7 @@
         <v>1</v>
       </c>
       <c r="I39" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J39">
         <v>2</v>
@@ -2153,7 +2153,7 @@
         <v>3</v>
       </c>
       <c r="L39" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
@@ -2161,7 +2161,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C40">
         <v>4</v>
@@ -2182,7 +2182,7 @@
         <v>1</v>
       </c>
       <c r="I40" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J40">
         <v>2</v>
@@ -2191,7 +2191,7 @@
         <v>3</v>
       </c>
       <c r="L40" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
@@ -2199,7 +2199,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C41">
         <v>4</v>
@@ -2220,7 +2220,7 @@
         <v>1</v>
       </c>
       <c r="I41" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J41">
         <v>2</v>
@@ -2229,7 +2229,7 @@
         <v>3</v>
       </c>
       <c r="L41" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
@@ -2237,7 +2237,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C42">
         <v>4</v>
@@ -2258,7 +2258,7 @@
         <v>1</v>
       </c>
       <c r="I42" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J42">
         <v>2</v>
@@ -2267,7 +2267,7 @@
         <v>3</v>
       </c>
       <c r="L42" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
@@ -2275,7 +2275,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C43">
         <v>4</v>
@@ -2296,7 +2296,7 @@
         <v>1</v>
       </c>
       <c r="I43" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J43">
         <v>2</v>
@@ -2305,7 +2305,7 @@
         <v>3</v>
       </c>
       <c r="L43" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
@@ -2313,7 +2313,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C44">
         <v>4</v>
@@ -2334,7 +2334,7 @@
         <v>1</v>
       </c>
       <c r="I44" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J44">
         <v>2</v>
@@ -2343,7 +2343,7 @@
         <v>3</v>
       </c>
       <c r="L44" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
@@ -2351,7 +2351,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C45">
         <v>4</v>
@@ -2372,7 +2372,7 @@
         <v>1</v>
       </c>
       <c r="I45" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J45">
         <v>2</v>
@@ -2381,7 +2381,7 @@
         <v>3</v>
       </c>
       <c r="L45" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
@@ -2389,7 +2389,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C46">
         <v>4</v>
@@ -2410,7 +2410,7 @@
         <v>1</v>
       </c>
       <c r="I46" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J46">
         <v>2</v>
@@ -2419,7 +2419,7 @@
         <v>3</v>
       </c>
       <c r="L46" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
@@ -2427,7 +2427,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C47">
         <v>4</v>
@@ -2448,7 +2448,7 @@
         <v>1</v>
       </c>
       <c r="I47" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J47">
         <v>2</v>
@@ -2457,7 +2457,7 @@
         <v>3</v>
       </c>
       <c r="L47" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
@@ -2465,7 +2465,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C48">
         <v>4</v>
@@ -2486,7 +2486,7 @@
         <v>1</v>
       </c>
       <c r="I48" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J48">
         <v>2</v>
@@ -2495,7 +2495,7 @@
         <v>3</v>
       </c>
       <c r="L48" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
@@ -2503,7 +2503,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C49">
         <v>4</v>
@@ -2524,7 +2524,7 @@
         <v>1</v>
       </c>
       <c r="I49" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J49">
         <v>2</v>
@@ -2533,7 +2533,7 @@
         <v>3</v>
       </c>
       <c r="L49" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
@@ -2541,7 +2541,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C50">
         <v>4</v>
@@ -2562,7 +2562,7 @@
         <v>1</v>
       </c>
       <c r="I50" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J50">
         <v>2</v>
@@ -2571,7 +2571,7 @@
         <v>3</v>
       </c>
       <c r="L50" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
@@ -2579,7 +2579,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C51">
         <v>4</v>
@@ -2600,7 +2600,7 @@
         <v>1</v>
       </c>
       <c r="I51" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J51">
         <v>2</v>
@@ -2609,7 +2609,7 @@
         <v>3</v>
       </c>
       <c r="L51" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
@@ -2617,7 +2617,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C52">
         <v>4</v>
@@ -2638,7 +2638,7 @@
         <v>1</v>
       </c>
       <c r="I52" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J52">
         <v>2</v>
@@ -2647,7 +2647,7 @@
         <v>3</v>
       </c>
       <c r="L52" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
@@ -2655,7 +2655,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C53">
         <v>4</v>
@@ -2676,7 +2676,7 @@
         <v>1</v>
       </c>
       <c r="I53" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J53">
         <v>2</v>
@@ -2685,7 +2685,7 @@
         <v>3</v>
       </c>
       <c r="L53" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
@@ -2693,7 +2693,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C54">
         <v>4</v>
@@ -2714,7 +2714,7 @@
         <v>1</v>
       </c>
       <c r="I54" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J54">
         <v>2</v>
@@ -2723,7 +2723,7 @@
         <v>3</v>
       </c>
       <c r="L54" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
@@ -2731,7 +2731,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C55">
         <v>4</v>
@@ -2752,7 +2752,7 @@
         <v>1</v>
       </c>
       <c r="I55" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J55">
         <v>2</v>
@@ -2761,7 +2761,7 @@
         <v>3</v>
       </c>
       <c r="L55" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
@@ -2769,7 +2769,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C56">
         <v>4</v>
@@ -2790,7 +2790,7 @@
         <v>1</v>
       </c>
       <c r="I56" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J56">
         <v>2</v>
@@ -2799,7 +2799,7 @@
         <v>3</v>
       </c>
       <c r="L56" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
@@ -2807,7 +2807,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C57">
         <v>4</v>
@@ -2828,7 +2828,7 @@
         <v>1</v>
       </c>
       <c r="I57" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J57">
         <v>2</v>
@@ -2837,7 +2837,7 @@
         <v>3</v>
       </c>
       <c r="L57" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
@@ -2845,7 +2845,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C58">
         <v>3</v>
@@ -2866,7 +2866,7 @@
         <v>1</v>
       </c>
       <c r="I58" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J58">
         <v>1</v>
@@ -2875,7 +2875,7 @@
         <v>3</v>
       </c>
       <c r="L58" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
@@ -2883,7 +2883,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C59">
         <v>3</v>
@@ -2904,7 +2904,7 @@
         <v>1</v>
       </c>
       <c r="I59" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J59">
         <v>1</v>
@@ -2913,7 +2913,7 @@
         <v>3</v>
       </c>
       <c r="L59" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
@@ -2921,7 +2921,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C60">
         <v>3</v>
@@ -2942,7 +2942,7 @@
         <v>1</v>
       </c>
       <c r="I60" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J60">
         <v>1</v>
@@ -2951,7 +2951,7 @@
         <v>3</v>
       </c>
       <c r="L60" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
@@ -2959,7 +2959,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C61">
         <v>3</v>
@@ -2980,7 +2980,7 @@
         <v>1</v>
       </c>
       <c r="I61" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J61">
         <v>1</v>
@@ -2989,7 +2989,7 @@
         <v>3</v>
       </c>
       <c r="L61" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
@@ -2997,7 +2997,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C62">
         <v>3</v>
@@ -3018,7 +3018,7 @@
         <v>1</v>
       </c>
       <c r="I62" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J62">
         <v>1</v>
@@ -3027,7 +3027,7 @@
         <v>3</v>
       </c>
       <c r="L62" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
@@ -3035,7 +3035,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C63">
         <v>3</v>
@@ -3056,7 +3056,7 @@
         <v>1</v>
       </c>
       <c r="I63" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J63">
         <v>1</v>
@@ -3065,7 +3065,7 @@
         <v>3</v>
       </c>
       <c r="L63" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
@@ -3073,7 +3073,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C64">
         <v>32</v>
@@ -3094,7 +3094,7 @@
         <v>1</v>
       </c>
       <c r="I64" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="J64">
         <v>1</v>
@@ -3103,7 +3103,7 @@
         <v>1</v>
       </c>
       <c r="L64" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
@@ -3111,7 +3111,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C65">
         <v>36</v>
@@ -3132,7 +3132,7 @@
         <v>1</v>
       </c>
       <c r="I65" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="J65">
         <v>1</v>
@@ -3141,7 +3141,7 @@
         <v>1</v>
       </c>
       <c r="L65" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
@@ -3149,7 +3149,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C66">
         <v>18</v>
@@ -3170,7 +3170,7 @@
         <v>1</v>
       </c>
       <c r="I66" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="J66">
         <v>1</v>
@@ -3179,7 +3179,7 @@
         <v>1</v>
       </c>
       <c r="L66" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
@@ -3187,7 +3187,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C67">
         <v>24</v>
@@ -3208,7 +3208,7 @@
         <v>1</v>
       </c>
       <c r="I67" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="J67">
         <v>1</v>
@@ -3217,7 +3217,7 @@
         <v>1</v>
       </c>
       <c r="L67" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.2">
@@ -3225,7 +3225,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C68">
         <v>15</v>
@@ -3246,7 +3246,7 @@
         <v>1</v>
       </c>
       <c r="I68" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="J68">
         <v>1</v>
@@ -3255,7 +3255,7 @@
         <v>1</v>
       </c>
       <c r="L68" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.2">
@@ -3263,7 +3263,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C69">
         <v>36</v>
@@ -3284,7 +3284,7 @@
         <v>1</v>
       </c>
       <c r="I69" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="J69">
         <v>1</v>
@@ -3293,7 +3293,7 @@
         <v>1</v>
       </c>
       <c r="L69" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -3308,8 +3308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81EC0AE1-86E2-6E4E-A8F7-D17753A03C2F}">
   <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" zoomScale="208" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView topLeftCell="A79" zoomScale="125" zoomScaleNormal="126" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3322,22 +3322,22 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -3354,7 +3354,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -3374,10 +3374,10 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -3394,7 +3394,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -3414,10 +3414,10 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -3434,7 +3434,7 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
@@ -3474,7 +3474,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -3494,10 +3494,10 @@
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -3514,10 +3514,10 @@
         <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -3534,10 +3534,10 @@
         <v>20</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -3554,10 +3554,10 @@
         <v>21</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -3574,10 +3574,10 @@
         <v>22</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -3594,10 +3594,10 @@
         <v>23</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -3614,10 +3614,10 @@
         <v>24</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -3634,10 +3634,10 @@
         <v>25</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -3654,10 +3654,10 @@
         <v>26</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -3674,10 +3674,10 @@
         <v>27</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -3694,10 +3694,10 @@
         <v>28</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -3714,10 +3714,10 @@
         <v>29</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -3734,10 +3734,10 @@
         <v>30</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -3754,10 +3754,10 @@
         <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -3774,10 +3774,10 @@
         <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -3794,10 +3794,10 @@
         <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -3814,10 +3814,10 @@
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -3834,10 +3834,10 @@
         <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D26" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -3854,10 +3854,10 @@
         <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="D27" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -3874,10 +3874,10 @@
         <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="D28" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -3894,10 +3894,10 @@
         <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D29" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -3914,10 +3914,10 @@
         <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D30" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -3934,10 +3934,10 @@
         <v>37</v>
       </c>
       <c r="C31" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D31" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -3954,10 +3954,10 @@
         <v>38</v>
       </c>
       <c r="C32" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -3974,10 +3974,10 @@
         <v>39</v>
       </c>
       <c r="C33" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D33" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -3994,10 +3994,10 @@
         <v>40</v>
       </c>
       <c r="C34" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D34" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -4014,10 +4014,10 @@
         <v>41</v>
       </c>
       <c r="C35" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D35" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -4034,10 +4034,10 @@
         <v>42</v>
       </c>
       <c r="C36" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D36" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -4054,10 +4054,10 @@
         <v>43</v>
       </c>
       <c r="C37" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D37" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -4074,10 +4074,10 @@
         <v>44</v>
       </c>
       <c r="C38" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D38" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -4094,10 +4094,10 @@
         <v>45</v>
       </c>
       <c r="C39" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D39" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -4114,10 +4114,10 @@
         <v>46</v>
       </c>
       <c r="C40" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D40" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -4134,10 +4134,10 @@
         <v>47</v>
       </c>
       <c r="C41" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D41" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -4154,10 +4154,10 @@
         <v>48</v>
       </c>
       <c r="C42" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D42" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E42">
         <v>1</v>
@@ -4174,10 +4174,10 @@
         <v>49</v>
       </c>
       <c r="C43" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D43" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E43">
         <v>1</v>
@@ -4194,10 +4194,10 @@
         <v>50</v>
       </c>
       <c r="C44" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D44" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -4214,10 +4214,10 @@
         <v>51</v>
       </c>
       <c r="C45" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D45" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -4234,10 +4234,10 @@
         <v>52</v>
       </c>
       <c r="C46" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D46" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E46">
         <v>1</v>
@@ -4254,10 +4254,10 @@
         <v>53</v>
       </c>
       <c r="C47" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D47" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -4274,10 +4274,10 @@
         <v>54</v>
       </c>
       <c r="C48" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D48" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -4294,10 +4294,10 @@
         <v>55</v>
       </c>
       <c r="C49" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E49">
         <v>1</v>
@@ -4314,10 +4314,10 @@
         <v>35</v>
       </c>
       <c r="C50" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D50" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E50">
         <v>1</v>
@@ -4334,10 +4334,10 @@
         <v>36</v>
       </c>
       <c r="C51" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D51" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E51">
         <v>1</v>
@@ -4354,10 +4354,10 @@
         <v>37</v>
       </c>
       <c r="C52" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D52" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E52">
         <v>1</v>
@@ -4374,10 +4374,10 @@
         <v>38</v>
       </c>
       <c r="C53" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D53" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E53">
         <v>1</v>
@@ -4394,10 +4394,10 @@
         <v>39</v>
       </c>
       <c r="C54" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D54" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E54">
         <v>1</v>
@@ -4414,10 +4414,10 @@
         <v>40</v>
       </c>
       <c r="C55" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D55" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E55">
         <v>1</v>
@@ -4434,10 +4434,10 @@
         <v>41</v>
       </c>
       <c r="C56" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D56" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -4454,10 +4454,10 @@
         <v>42</v>
       </c>
       <c r="C57" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D57" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E57">
         <v>1</v>
@@ -4474,10 +4474,10 @@
         <v>43</v>
       </c>
       <c r="C58" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D58" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -4494,10 +4494,10 @@
         <v>44</v>
       </c>
       <c r="C59" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D59" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E59">
         <v>1</v>
@@ -4514,10 +4514,10 @@
         <v>45</v>
       </c>
       <c r="C60" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D60" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E60">
         <v>1</v>
@@ -4534,10 +4534,10 @@
         <v>46</v>
       </c>
       <c r="C61" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D61" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -4554,10 +4554,10 @@
         <v>47</v>
       </c>
       <c r="C62" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D62" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -4574,10 +4574,10 @@
         <v>48</v>
       </c>
       <c r="C63" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D63" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E63">
         <v>1</v>
@@ -4594,10 +4594,10 @@
         <v>49</v>
       </c>
       <c r="C64" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D64" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E64">
         <v>1</v>
@@ -4614,10 +4614,10 @@
         <v>50</v>
       </c>
       <c r="C65" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D65" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E65">
         <v>1</v>
@@ -4634,10 +4634,10 @@
         <v>51</v>
       </c>
       <c r="C66" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D66" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E66">
         <v>1</v>
@@ -4654,10 +4654,10 @@
         <v>52</v>
       </c>
       <c r="C67" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D67" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E67">
         <v>1</v>
@@ -4674,10 +4674,10 @@
         <v>53</v>
       </c>
       <c r="C68" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D68" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E68">
         <v>1</v>
@@ -4694,10 +4694,10 @@
         <v>54</v>
       </c>
       <c r="C69" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D69" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -4714,10 +4714,10 @@
         <v>55</v>
       </c>
       <c r="C70" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D70" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E70">
         <v>1</v>
@@ -4734,10 +4734,10 @@
         <v>17</v>
       </c>
       <c r="C71" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D71" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E71">
         <v>1</v>
@@ -4754,10 +4754,10 @@
         <v>17</v>
       </c>
       <c r="C72" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D72" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -4774,10 +4774,10 @@
         <v>17</v>
       </c>
       <c r="C73" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D73" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E73">
         <v>1</v>
@@ -4794,10 +4794,10 @@
         <v>17</v>
       </c>
       <c r="C74" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D74" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E74">
         <v>1</v>
@@ -4814,10 +4814,10 @@
         <v>17</v>
       </c>
       <c r="C75" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D75" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E75">
         <v>1</v>
@@ -4834,10 +4834,10 @@
         <v>17</v>
       </c>
       <c r="C76" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D76" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E76">
         <v>1</v>
@@ -4854,10 +4854,10 @@
         <v>17</v>
       </c>
       <c r="C77" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D77" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E77">
         <v>1</v>
@@ -4874,10 +4874,10 @@
         <v>17</v>
       </c>
       <c r="C78" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D78" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E78">
         <v>1</v>
@@ -4894,10 +4894,10 @@
         <v>17</v>
       </c>
       <c r="C79" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D79" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E79">
         <v>1</v>
@@ -4914,10 +4914,10 @@
         <v>17</v>
       </c>
       <c r="C80" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D80" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E80">
         <v>1</v>
@@ -4934,10 +4934,10 @@
         <v>17</v>
       </c>
       <c r="C81" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D81" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E81">
         <v>1</v>
@@ -4954,10 +4954,10 @@
         <v>17</v>
       </c>
       <c r="C82" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D82" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E82">
         <v>1</v>
@@ -4974,10 +4974,10 @@
         <v>17</v>
       </c>
       <c r="C83" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D83" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E83">
         <v>1</v>
@@ -4994,10 +4994,10 @@
         <v>17</v>
       </c>
       <c r="C84" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D84" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E84">
         <v>1</v>
@@ -5014,10 +5014,10 @@
         <v>17</v>
       </c>
       <c r="C85" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D85" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E85">
         <v>1</v>
@@ -5034,10 +5034,10 @@
         <v>17</v>
       </c>
       <c r="C86" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D86" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E86">
         <v>1</v>
@@ -5054,10 +5054,10 @@
         <v>17</v>
       </c>
       <c r="C87" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D87" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E87">
         <v>1</v>
@@ -5074,10 +5074,10 @@
         <v>17</v>
       </c>
       <c r="C88" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D88" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E88">
         <v>1</v>
@@ -5094,10 +5094,10 @@
         <v>17</v>
       </c>
       <c r="C89" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D89" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E89">
         <v>1</v>
@@ -5114,10 +5114,10 @@
         <v>17</v>
       </c>
       <c r="C90" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D90" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E90">
         <v>1</v>
@@ -5134,10 +5134,10 @@
         <v>17</v>
       </c>
       <c r="C91" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D91" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E91">
         <v>1</v>
@@ -5154,10 +5154,10 @@
         <v>66</v>
       </c>
       <c r="C92" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="D92" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E92">
         <v>1</v>
@@ -5174,10 +5174,10 @@
         <v>65</v>
       </c>
       <c r="C93" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="D93" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E93">
         <v>1</v>
@@ -5194,10 +5194,10 @@
         <v>65</v>
       </c>
       <c r="C94" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="D94" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E94">
         <v>1</v>
@@ -5214,10 +5214,10 @@
         <v>65</v>
       </c>
       <c r="C95" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="D95" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E95">
         <v>1</v>
@@ -5234,10 +5234,10 @@
         <v>64</v>
       </c>
       <c r="C96" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="D96" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E96">
         <v>1</v>
@@ -5254,10 +5254,10 @@
         <v>63</v>
       </c>
       <c r="C97" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="D97" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E97">
         <v>1</v>
@@ -5274,10 +5274,10 @@
         <v>62</v>
       </c>
       <c r="C98" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="D98" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E98">
         <v>1</v>
@@ -5294,10 +5294,10 @@
         <v>34</v>
       </c>
       <c r="C99" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="D99" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E99">
         <v>1</v>
@@ -5314,10 +5314,10 @@
         <v>67</v>
       </c>
       <c r="C100" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="D100" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E100">
         <v>1</v>
@@ -5334,10 +5334,10 @@
         <v>34</v>
       </c>
       <c r="C101" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="D101" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E101">
         <v>1</v>
@@ -5354,10 +5354,10 @@
         <v>33</v>
       </c>
       <c r="C102" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="D102" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E102">
         <v>1</v>
@@ -5374,10 +5374,10 @@
         <v>63</v>
       </c>
       <c r="C103" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="D103" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E103">
         <v>1</v>
@@ -5400,7 +5400,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView zoomScale="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B33"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5411,22 +5411,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -5457,10 +5457,10 @@
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -5477,10 +5477,10 @@
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -5497,10 +5497,10 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -5517,10 +5517,10 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -5537,10 +5537,10 @@
         <v>32</v>
       </c>
       <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
         <v>32</v>
-      </c>
-      <c r="D7" t="s">
-        <v>35</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -5557,10 +5557,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -5577,7 +5577,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -5597,10 +5597,10 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -5617,10 +5617,10 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -5637,10 +5637,10 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -5657,10 +5657,10 @@
         <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -5677,10 +5677,10 @@
         <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -5697,10 +5697,10 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -5717,10 +5717,10 @@
         <v>2</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -5737,10 +5737,10 @@
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -5757,10 +5757,10 @@
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -5777,10 +5777,10 @@
         <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -5797,10 +5797,10 @@
         <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -5817,10 +5817,10 @@
         <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D21" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -5837,10 +5837,10 @@
         <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D22" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -5857,10 +5857,10 @@
         <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D23" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -5877,10 +5877,10 @@
         <v>42</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D24" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -5897,10 +5897,10 @@
         <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D25" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -5917,10 +5917,10 @@
         <v>45</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D26" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -5937,10 +5937,10 @@
         <v>46</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D27" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -5957,10 +5957,10 @@
         <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D28" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -5977,10 +5977,10 @@
         <v>50</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -5997,10 +5997,10 @@
         <v>51</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D30" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -6017,10 +6017,10 @@
         <v>53</v>
       </c>
       <c r="C31" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D31" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -6037,10 +6037,10 @@
         <v>54</v>
       </c>
       <c r="C32" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D32" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -6057,10 +6057,10 @@
         <v>55</v>
       </c>
       <c r="C33" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D33" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E33">
         <v>1</v>

</xml_diff>